<commit_message>
planilhas para data análises.
</commit_message>
<xml_diff>
--- a/Data Science Introdução a análise de series temporais/Series Temporais data-analysis-a3.xlsx
+++ b/Data Science Introdução a análise de series temporais/Series Temporais data-analysis-a3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wcamentoring-my.sharepoint.com/personal/alexsandro_ignacio_wca-ec_com_br/Documents/Documentos/Docs/Git/python_developer/Data Science Introdução a análise de series temporais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_6D6D3A00E23BC08A8658563FBD17460E90AB451C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66DA4AE3-136E-4F18-B75B-74CA5B0A2A15}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="11_6D6D3A00E23BC08A8658563FBD17460E90AB451C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69EDDEBA-6B0D-406D-B156-50F37E016525}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="450" yWindow="1005" windowWidth="20490" windowHeight="10155" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="660" yWindow="180" windowWidth="17475" windowHeight="10740" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brancos" sheetId="1" r:id="rId1"/>
@@ -8328,7 +8328,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -8360,7 +8360,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -8447,7 +8447,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -8479,7 +8479,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -9195,7 +9195,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -9227,7 +9227,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -10534,7 +10534,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -10566,7 +10566,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -10653,7 +10653,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -10685,7 +10685,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -11456,7 +11456,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -11488,7 +11488,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -12225,7 +12225,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -12257,7 +12257,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -12345,7 +12345,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -12377,7 +12377,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -26529,8 +26529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E28" sqref="C1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26538,9 +26538,10 @@
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="17" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="17" width="14.42578125" customWidth="1"/>
     <col min="18" max="18" width="13.42578125" customWidth="1"/>
     <col min="19" max="1025" width="14.42578125" customWidth="1"/>
   </cols>
@@ -28267,7 +28268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -50837,11 +50838,11 @@
       </c>
       <c r="G1">
         <f t="array" aca="1" ref="G1:H1" ca="1">LINEST(E2:E37)</f>
-        <v>5.6353904207099701</v>
+        <v>5.6354692504364419</v>
       </c>
       <c r="H1">
         <f ca="1"/>
-        <v>6.1412195624196073</v>
+        <v>5.9388775713238999</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -50856,22 +50857,22 @@
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D37" ca="1" si="0">RAND()*5</f>
-        <v>2.1284724470322769</v>
+        <v>7.9403064622659003E-2</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E37" ca="1" si="1">B2*C2+D2</f>
-        <v>12.128472447032276</v>
+        <v>10.079403064622658</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G37" ca="1" si="2">$H$1+(F2*$G$1)</f>
-        <v>11.776609983129578</v>
+        <v>11.574346821760342</v>
       </c>
       <c r="H2" s="7">
         <f t="shared" ref="H2:H37" ca="1" si="3">E2-G2</f>
-        <v>0.35186246390269815</v>
+        <v>-1.4949437571376833</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -50886,22 +50887,22 @@
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8288413426639494</v>
+        <v>0.35552938810395451</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>21.828841342663949</v>
+        <v>18.355529388103953</v>
       </c>
       <c r="F3" s="7">
         <v>2</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="2"/>
-        <v>17.412000403839549</v>
+        <v>17.209816072196784</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4168409388244001</v>
+        <v>1.1457133159071695</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -50916,22 +50917,22 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7216489830019954</v>
+        <v>3.8189103303942269</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>27.721648983001995</v>
+        <v>29.818910330394228</v>
       </c>
       <c r="F4" s="7">
         <v>3</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="2"/>
-        <v>23.047390824549517</v>
+        <v>22.845285322633224</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>4.6742581584524778</v>
+        <v>6.9736250077610045</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -50946,22 +50947,22 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.176109326435113</v>
+        <v>2.8810319102334652</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>21.176109326435114</v>
+        <v>22.881031910233464</v>
       </c>
       <c r="F5" s="7">
         <v>4</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="2"/>
-        <v>28.682781245259488</v>
+        <v>28.480754573069667</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-7.5066719188243738</v>
+        <v>-5.5997226628362036</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -50976,22 +50977,22 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4812765501181944</v>
+        <v>0.76781076816032467</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>29.481276550118196</v>
+        <v>27.767810768160324</v>
       </c>
       <c r="F6" s="7">
         <v>5</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="2"/>
-        <v>34.318171665969459</v>
+        <v>34.116223823506111</v>
       </c>
       <c r="H6" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.836895115851263</v>
+        <v>-6.3484130553457874</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51006,22 +51007,22 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70291750648405926</v>
+        <v>0.55403405938289629</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>35.702917506484056</v>
+        <v>35.554034059382893</v>
       </c>
       <c r="F7" s="7">
         <v>6</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="2"/>
-        <v>39.953562086679426</v>
+        <v>39.751693073942548</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.2506445801953703</v>
+        <v>-4.1976590145596546</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51036,22 +51037,22 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2189522823322609</v>
+        <v>2.0525478691296017</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>62.21895228233226</v>
+        <v>62.052547869129604</v>
       </c>
       <c r="F8" s="7">
         <v>7</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="2"/>
-        <v>45.588952507389401</v>
+        <v>45.387162324378991</v>
       </c>
       <c r="H8" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>16.62999977494286</v>
+        <v>16.665385544750613</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51066,22 +51067,22 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10894797288349689</v>
+        <v>2.3592418573061895</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>54.108947972883499</v>
+        <v>56.359241857306188</v>
       </c>
       <c r="F9" s="7">
         <v>8</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
-        <v>51.224342928099368</v>
+        <v>51.022631574815435</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8846050447841307</v>
+        <v>5.3366102824907529</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51096,22 +51097,22 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.394856236938371</v>
+        <v>2.8437314554657926</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>51.394856236938374</v>
+        <v>52.843731455465793</v>
       </c>
       <c r="F10" s="7">
         <v>9</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="2"/>
-        <v>56.859733348809335</v>
+        <v>56.658100825251879</v>
       </c>
       <c r="H10" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-5.4648771118709618</v>
+        <v>-3.8143693697860854</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51126,22 +51127,22 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1733195119931978</v>
+        <v>2.9526742779659192</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>56.173319511993199</v>
+        <v>57.952674277965919</v>
       </c>
       <c r="F11" s="7">
         <v>10</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="2"/>
-        <v>62.49512376951931</v>
+        <v>62.293570075688322</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-6.3218042575261109</v>
+        <v>-4.3408957977224034</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51156,22 +51157,22 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9638820490908189</v>
+        <v>0.4479206868499136</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>49.96388204909082</v>
+        <v>48.447920686849912</v>
       </c>
       <c r="F12" s="7">
         <v>11</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="2"/>
-        <v>68.130514190229277</v>
+        <v>67.929039326124752</v>
       </c>
       <c r="H12" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-18.166632141138457</v>
+        <v>-19.48111863927484</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51186,22 +51187,22 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61329763406129556</v>
+        <v>1.387687038676938</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>98.113297634061297</v>
+        <v>98.887687038676944</v>
       </c>
       <c r="F13" s="7">
         <v>12</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="2"/>
-        <v>73.765904610939245</v>
+        <v>73.564508576561195</v>
       </c>
       <c r="H13" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>24.347393023122052</v>
+        <v>25.323178462115749</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51216,22 +51217,22 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5664926775409667</v>
+        <v>1.0625499784156678</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>74.566492677540964</v>
+        <v>71.062549978415674</v>
       </c>
       <c r="F14" s="7">
         <v>13</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="2"/>
-        <v>79.401295031649212</v>
+        <v>79.199977826997639</v>
       </c>
       <c r="H14" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.8348023541082483</v>
+        <v>-8.1374278485819644</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51246,22 +51247,22 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>3.531748372976018</v>
+        <v>3.1366132369153279</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>93.531748372976011</v>
+        <v>93.136613236915323</v>
       </c>
       <c r="F15" s="7">
         <v>14</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="2"/>
-        <v>85.036685452359194</v>
+        <v>84.835447077434083</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>8.4950629206168173</v>
+        <v>8.3011661594812409</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51276,22 +51277,22 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9335752461199869</v>
+        <v>4.1823483835427959</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>108.93357524611999</v>
+        <v>108.1823483835428</v>
       </c>
       <c r="F16" s="7">
         <v>15</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="2"/>
-        <v>90.672075873069161</v>
+        <v>90.470916327870526</v>
       </c>
       <c r="H16" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>18.261499373050825</v>
+        <v>17.711432055672276</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51306,22 +51307,22 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3909766706249709</v>
+        <v>1.9410348581565247</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>69.390976670624966</v>
+        <v>69.941034858156527</v>
       </c>
       <c r="F17" s="7">
         <v>16</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="2"/>
-        <v>96.307466293779129</v>
+        <v>96.10638557830697</v>
       </c>
       <c r="H17" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-26.916489623154163</v>
+        <v>-26.165350720150442</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51336,22 +51337,22 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9653977981530897</v>
+        <v>4.1314665504789021</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>85.965397798153091</v>
+        <v>85.131466550478905</v>
       </c>
       <c r="F18" s="7">
         <v>17</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="2"/>
-        <v>101.9428567144891</v>
+        <v>101.74185482874341</v>
       </c>
       <c r="H18" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-15.977458916336005</v>
+        <v>-16.610388278264509</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51366,22 +51367,22 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4389320929087925</v>
+        <v>3.2980579228797779</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>98.438932092908786</v>
+        <v>98.298057922879778</v>
       </c>
       <c r="F19" s="7">
         <v>18</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="2"/>
-        <v>107.57824713519906</v>
+        <v>107.37732407917986</v>
       </c>
       <c r="H19" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-9.1393150422902778</v>
+        <v>-9.0792661563000792</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51396,22 +51397,22 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5233654160431431</v>
+        <v>3.7479383868574763</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>154.52336541604313</v>
+        <v>153.74793838685747</v>
       </c>
       <c r="F20" s="7">
         <v>19</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="2"/>
-        <v>113.21363755590905</v>
+        <v>113.0127933296163</v>
       </c>
       <c r="H20" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>41.309727860134089</v>
+        <v>40.735145057241169</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51426,22 +51427,22 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7051820462352598</v>
+        <v>4.126038997651218</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>130.70518204623525</v>
+        <v>130.12603899765122</v>
       </c>
       <c r="F21" s="7">
         <v>20</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="2"/>
-        <v>118.84902797661901</v>
+        <v>118.64826258005274</v>
       </c>
       <c r="H21" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>11.856154069616238</v>
+        <v>11.477776417598477</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51456,22 +51457,22 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1643987822762247</v>
+        <v>3.8872020624352559</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>111.16439878227622</v>
+        <v>113.88720206243525</v>
       </c>
       <c r="F22" s="7">
         <v>21</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="2"/>
-        <v>124.48441839732898</v>
+        <v>124.28373183048917</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-13.320019615052757</v>
+        <v>-10.396529768053924</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51486,22 +51487,22 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0664887438570796</v>
+        <v>0.94091553179175891</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>117.06648874385708</v>
+        <v>115.94091553179176</v>
       </c>
       <c r="F23" s="7">
         <v>22</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="2"/>
-        <v>130.11980881803896</v>
+        <v>129.91920108092563</v>
       </c>
       <c r="H23" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-13.053320074181883</v>
+        <v>-13.978285549133872</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51516,22 +51517,22 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9048571852321867</v>
+        <v>3.5505594487928294</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>100.90485718523219</v>
+        <v>99.550559448792825</v>
       </c>
       <c r="F24" s="7">
         <v>23</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="2"/>
-        <v>135.7551992387489</v>
+        <v>135.55467033136208</v>
       </c>
       <c r="H24" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-34.850342053516712</v>
+        <v>-36.00411088256925</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51546,22 +51547,22 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2602636972754935</v>
+        <v>1.2069169069252106</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>191.76026369727549</v>
+        <v>188.70691690692522</v>
       </c>
       <c r="F25" s="7">
         <v>24</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="2"/>
-        <v>141.3905896594589</v>
+        <v>141.19013958179849</v>
       </c>
       <c r="H25" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>50.369674037816594</v>
+        <v>47.516777325126725</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51576,22 +51577,22 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28930502542477754</v>
+        <v>4.063575555192255</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>130.28930502542477</v>
+        <v>134.06357555519224</v>
       </c>
       <c r="F26" s="7">
         <v>25</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="2"/>
-        <v>147.02598008016884</v>
+        <v>146.82560883223493</v>
       </c>
       <c r="H26" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-16.736675054744069</v>
+        <v>-12.76203327704269</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51606,22 +51607,22 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4578574657727392</v>
+        <v>4.1981446797366635</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>166.45785746577275</v>
+        <v>166.19814467973666</v>
       </c>
       <c r="F27" s="7">
         <v>26</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="2"/>
-        <v>152.66137050087883</v>
+        <v>152.46107808267138</v>
       </c>
       <c r="H27" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>13.796486964893916</v>
+        <v>13.737066597065279</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51636,22 +51637,22 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74718535808387776</v>
+        <v>2.5151963795091907</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>182.74718535808387</v>
+        <v>184.51519637950918</v>
       </c>
       <c r="F28" s="7">
         <v>27</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="2"/>
-        <v>158.29676092158883</v>
+        <v>158.09654733310782</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>24.450424436495041</v>
+        <v>26.418649046401356</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51666,22 +51667,22 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2616472489237225</v>
+        <v>3.2372436107341285</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>118.26164724892372</v>
+        <v>119.23724361073413</v>
       </c>
       <c r="F29" s="7">
         <v>28</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="2"/>
-        <v>163.93215134229877</v>
+        <v>163.73201658354427</v>
       </c>
       <c r="H29" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-45.670504093375044</v>
+        <v>-44.494772972810139</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51696,22 +51697,22 @@
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4444625776397011</v>
+        <v>3.0266040525904274</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>137.44446257763971</v>
+        <v>138.02660405259041</v>
       </c>
       <c r="F30" s="7">
         <v>29</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="2"/>
-        <v>169.56754176300876</v>
+        <v>169.36748583398071</v>
       </c>
       <c r="H30" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-32.12307918536905</v>
+        <v>-31.340881781390294</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51726,22 +51727,22 @@
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2740419052262575</v>
+        <v>0.56761895799256334</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="1"/>
-        <v>156.27404190522626</v>
+        <v>155.56761895799255</v>
       </c>
       <c r="F31" s="7">
         <v>30</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="2"/>
-        <v>175.2029321837187</v>
+        <v>175.00295508441715</v>
       </c>
       <c r="H31" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-18.928890278492446</v>
+        <v>-19.435336126424602</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51756,22 +51757,22 @@
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5244968597105748</v>
+        <v>2.3999513817275941</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="1"/>
-        <v>244.52449685971058</v>
+        <v>242.39995138172759</v>
       </c>
       <c r="F32" s="7">
         <v>31</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="2"/>
-        <v>180.8383226044287</v>
+        <v>180.6384243348536</v>
       </c>
       <c r="H32" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>63.686174255281884</v>
+        <v>61.761527046873994</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51786,22 +51787,22 @@
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8539775036949324</v>
+        <v>3.0340567985115117</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="1"/>
-        <v>202.85397750369492</v>
+        <v>201.0340567985115</v>
       </c>
       <c r="F33" s="7">
         <v>32</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="2"/>
-        <v>186.47371302513864</v>
+        <v>186.27389358529004</v>
       </c>
       <c r="H33" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>16.380264478556285</v>
+        <v>14.76016321322146</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51816,22 +51817,22 @@
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5141012366253825</v>
+        <v>2.2785052923342648</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="1"/>
-        <v>174.51410123662538</v>
+        <v>172.27850529233427</v>
       </c>
       <c r="F34" s="7">
         <v>33</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="2"/>
-        <v>192.10910344584863</v>
+        <v>191.90936283572648</v>
       </c>
       <c r="H34" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-17.595002209223253</v>
+        <v>-19.63085754339221</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51846,22 +51847,22 @@
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5566017623047386</v>
+        <v>3.92575969274895</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="1"/>
-        <v>178.55660176230475</v>
+        <v>178.92575969274895</v>
       </c>
       <c r="F35" s="7">
         <v>34</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="2"/>
-        <v>197.74449386655857</v>
+        <v>197.54483208616293</v>
       </c>
       <c r="H35" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-19.18789210425382</v>
+        <v>-18.619072393413973</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51876,22 +51877,22 @@
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5467901113211782</v>
+        <v>0.50595758005255453</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="1"/>
-        <v>146.54679011132117</v>
+        <v>144.50595758005255</v>
       </c>
       <c r="F36" s="7">
         <v>35</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="2"/>
-        <v>203.37988428726857</v>
+        <v>203.18030133659937</v>
       </c>
       <c r="H36" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>-56.833094175947394</v>
+        <v>-58.674343756546818</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
@@ -51906,22 +51907,22 @@
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="0"/>
-        <v>1.319256812941092</v>
+        <v>4.0573344060669463</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="1"/>
-        <v>278.81925681294109</v>
+        <v>281.55733440606696</v>
       </c>
       <c r="F37" s="7">
         <v>36</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="2"/>
-        <v>209.01527470797851</v>
+        <v>208.81577058703581</v>
       </c>
       <c r="H37" s="7">
         <f t="shared" ca="1" si="3"/>
-        <v>69.803982104962586</v>
+        <v>72.741563819031143</v>
       </c>
     </row>
     <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>